<commit_message>
add unit in bulk
</commit_message>
<xml_diff>
--- a/web/templates/add-unit-template.xlsx
+++ b/web/templates/add-unit-template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuhan\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yii2_stok_barang\web\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18D7B884-81F2-48C1-B452-FC63EACE244C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53397EEC-8FF3-4C74-9C82-31BAD7E0E0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{732D6342-8BE7-4639-A766-7FF72DF9C6DC}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>SKU</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>id_wh</t>
   </si>
@@ -48,9 +45,6 @@
   </si>
   <si>
     <t>comment</t>
-  </si>
-  <si>
-    <t>Item's SKU</t>
   </si>
   <si>
     <t>warehouse's id</t>
@@ -431,21 +425,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685BB158-DD99-4891-9DA2-7E37A48E1785}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="43.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,22 +448,16 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
qol changes main inventory - item detail - edit unit button added main inv - item detail - dropdown option for filter unit log - filter moved from gridview, date range filter added add unit - bulk - preview data before save add unit bulk - document saved and uploaded view list of all uploaded bulk add unit document download list of all uploaded bulk add unit document
</commit_message>
<xml_diff>
--- a/web/templates/add-unit-template.xlsx
+++ b/web/templates/add-unit-template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\yii2_stok_barang\web\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53397EEC-8FF3-4C74-9C82-31BAD7E0E0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A1362A-3FE3-4284-9F2C-A39EAA15E6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{732D6342-8BE7-4639-A766-7FF72DF9C6DC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>id_wh</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>comment about unit. Will autogenerate if empty</t>
+  </si>
+  <si>
+    <t>example below</t>
+  </si>
+  <si>
+    <t>empty serial number. Serial number will auto generate</t>
+  </si>
+  <si>
+    <t>HGPS-123</t>
+  </si>
+  <si>
+    <t>serial number not empty. Will not autogenerate</t>
+  </si>
+  <si>
+    <t>Comment content here</t>
   </si>
 </sst>
 </file>
@@ -425,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685BB158-DD99-4891-9DA2-7E37A48E1785}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +475,38 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>